<commit_message>
add sorting data fiture
</commit_message>
<xml_diff>
--- a/uploads/template_user.xlsx
+++ b/uploads/template_user.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50" count="50">
   <si>
     <t>No.Pegawai</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t>IV/e, Pembina Utama</t>
+  </si>
+  <si>
+    <t>ffgrt</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>JENIS KELAMIN</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -235,15 +256,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
-      <alignment vertical="top"/>
+      <alignment vertical="bottom"/>
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0">
-      <alignment vertical="top"/>
+      <alignment vertical="bottom"/>
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0">
-      <alignment vertical="top"/>
+      <alignment vertical="bottom"/>
       <protection locked="0" hidden="0"/>
     </xf>
   </cellStyleXfs>
@@ -566,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:O13"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="P1">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" defaultColWidth="10"/>
@@ -589,7 +610,8 @@
     <col min="14" max="14" customWidth="1" width="47.85547" style="0"/>
     <col min="15" max="15" customWidth="1" width="7.4257812" style="0"/>
     <col min="17" max="17" customWidth="1" width="33.0" style="0"/>
-    <col min="18" max="18" customWidth="1" width="6.140625" style="0"/>
+    <col min="18" max="18" customWidth="1" width="7.6992188" style="0"/>
+    <col min="20" max="20" customWidth="1" width="19.597656" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="8:8" ht="45.75" customHeight="1">
@@ -641,74 +663,94 @@
       <c r="R1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="8:8" ht="15.0">
+      <c r="T1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="8:8" ht="15.45">
+      <c r="B2"/>
       <c r="N2"/>
       <c r="O2" s="4"/>
       <c r="Q2"/>
       <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="8:8" ht="15.0">
+      <c r="T2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="8:8" ht="15.45">
+      <c r="B3"/>
       <c r="N3"/>
       <c r="O3" s="4"/>
       <c r="Q3"/>
       <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="8:8" ht="15.0">
+      <c r="T3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="8:8">
       <c r="N4"/>
       <c r="O4" s="4"/>
       <c r="Q4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="8:8" ht="15.0">
+    <row r="5" spans="8:8">
       <c r="N5"/>
       <c r="O5" s="4"/>
       <c r="Q5"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="8:8" ht="15.0">
+    <row r="6" spans="8:8">
       <c r="N6"/>
       <c r="O6" s="4"/>
       <c r="Q6"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="8:8" ht="15.0">
+    <row r="7" spans="8:8">
       <c r="N7"/>
       <c r="O7" s="4"/>
       <c r="Q7"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="8:8" ht="15.0">
+    <row r="8" spans="8:8">
       <c r="N8"/>
       <c r="O8" s="4"/>
       <c r="Q8"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="8:8" ht="15.0">
+    <row r="9" spans="8:8">
       <c r="N9"/>
       <c r="O9" s="4"/>
       <c r="Q9"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="8:8" ht="15.0">
+    <row r="10" spans="8:8">
       <c r="N10"/>
       <c r="O10" s="4"/>
       <c r="Q10"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="8:8" ht="15.0">
+    <row r="11" spans="8:8">
       <c r="N11"/>
       <c r="O11" s="4"/>
       <c r="Q11"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="8:8" ht="15.0">
+    <row r="12" spans="8:8">
       <c r="N12"/>
       <c r="O12" s="4"/>
       <c r="Q12"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="8:8" ht="15.0">
+    <row r="13" spans="8:8">
       <c r="N13"/>
       <c r="O13" s="4"/>
       <c r="Q13"/>
@@ -741,7 +783,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>

</xml_diff>